<commit_message>
Work more through Udacity Inferential Stats, EDX UCSD, and Udemy SQL
</commit_message>
<xml_diff>
--- a/Stats/Udacity/DataAnalystNanoDegree/IntroToInferentialStats/Lesson7_1WayANOVA.xlsx
+++ b/Stats/Udacity/DataAnalystNanoDegree/IntroToInferentialStats/Lesson7_1WayANOVA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
   <si>
     <t xml:space="preserve">alpha </t>
   </si>
@@ -81,6 +81,18 @@
   </si>
   <si>
     <t>F is w/in F-crit =reject h(0) = at least 2 stores have significantly diffferent prices</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Twin</t>
+  </si>
+  <si>
+    <t>Triplet</t>
+  </si>
+  <si>
+    <t>F is w/in F-crit = reject h(0) = twins children may show slower language development than gisnlfe children, and triplets are even slower</t>
   </si>
 </sst>
 </file>
@@ -502,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X46"/>
+  <dimension ref="A1:X47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,132 +912,496 @@
       <c r="J16" s="4"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" spans="8:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I17" s="4"/>
       <c r="J17" s="3"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="8:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I18" s="4"/>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="8:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="4"/>
+    <row r="18" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="19" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="1">
+        <f>AVERAGE(A19:C23)</f>
+        <v>6</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="8">
+        <f>COUNT(A24:C24)-1</f>
+        <v>2</v>
+      </c>
       <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="8:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I20" s="4"/>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="24" spans="8:20" x14ac:dyDescent="0.25">
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="8:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="T25" s="1"/>
-    </row>
-    <row r="26" spans="8:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="1">
+        <f>COUNT(C19:C23)</f>
+        <v>5</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="9">
+        <f>COUNT(A19:C23)-COUNT(A24:C24)</f>
+        <v>12</v>
+      </c>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="1">
+        <f>F20*SUM(E27:G27)</f>
+        <v>40</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="9">
+        <f>F21/I19</f>
+        <v>20</v>
+      </c>
+      <c r="J21" s="4"/>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="1">
+        <f>SUM(E30:G34)</f>
+        <v>42</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="9">
+        <f>F22/I20</f>
+        <v>3.5</v>
+      </c>
+      <c r="J22" s="4"/>
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="4"/>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <f>AVERAGE(A19:A23)</f>
+        <v>8</v>
+      </c>
+      <c r="B24" s="1">
+        <f>AVERAGE(B19:B23)</f>
+        <v>6</v>
+      </c>
+      <c r="C24" s="1">
+        <f>AVERAGE(C19:C23)</f>
+        <v>4</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="H24" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="9">
+        <f>I21/I22</f>
+        <v>5.7142857142857144</v>
+      </c>
+      <c r="J24" s="4"/>
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="1"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
       <c r="R26" s="1"/>
       <c r="T26" s="1"/>
     </row>
-    <row r="27" spans="8:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
+    <row r="27" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f>A24-$F$19</f>
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <f>B24-$F$19</f>
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <f>C24-$F$19</f>
+        <v>-2</v>
+      </c>
+      <c r="E27">
+        <f>A27^2</f>
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <f>B27^2</f>
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f>C27^2</f>
+        <v>4</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="9">
+        <v>3.8853</v>
+      </c>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
       <c r="R27" s="1"/>
-    </row>
-    <row r="28" spans="8:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
+      <c r="T27" s="1"/>
+    </row>
+    <row r="28" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="8:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="R29" s="1"/>
-    </row>
-    <row r="30" spans="8:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="Q30" s="1"/>
+    <row r="29" spans="1:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="I29" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
+    </row>
+    <row r="30" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f>A19-$A$24</f>
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <f>B19-$B$24</f>
+        <v>-2</v>
+      </c>
+      <c r="C30">
+        <f>C19-$C$24</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="2">
+        <f>A30^2</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" ref="F30:F33" si="6">B30^2</f>
+        <v>4</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" ref="G30:G33" si="7">C30^2</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="8:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
+    <row r="31" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" ref="A31:A34" si="8">A20-$A$24</f>
+        <v>-1</v>
+      </c>
+      <c r="B31">
+        <f t="shared" ref="B31:B34" si="9">B20-$B$24</f>
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <f t="shared" ref="C31:C34" si="10">C20-$C$24</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" ref="E31:E33" si="11">A31^2</f>
+        <v>1</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="8:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
+    <row r="32" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" spans="5:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N33" s="4"/>
+    <row r="33" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" si="8"/>
+        <v>-2</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="9"/>
+        <v>-2</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="10"/>
+        <v>-2</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="5:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N34" s="4"/>
+    <row r="34" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="10"/>
+        <v>-1</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" ref="E34" si="12">A34^2</f>
+        <v>1</v>
+      </c>
+      <c r="F34" s="2">
+        <f t="shared" ref="F34" si="13">B34^2</f>
+        <v>9</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" ref="G34" si="14">C34^2</f>
+        <v>1</v>
+      </c>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="M34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
     </row>
-    <row r="35" spans="5:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
+    <row r="35" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E35" s="1">
+        <f>SUM(E30:E34)</f>
+        <v>10</v>
+      </c>
+      <c r="F35" s="1">
+        <f t="shared" ref="F35:G35" si="15">SUM(F30:F34)</f>
+        <v>18</v>
+      </c>
+      <c r="G35" s="1">
+        <f t="shared" si="15"/>
+        <v>14</v>
+      </c>
       <c r="N35" s="4"/>
-      <c r="Q35" s="2"/>
-      <c r="R35" s="2"/>
-    </row>
-    <row r="36" spans="5:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+    </row>
+    <row r="36" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="N36" s="4"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
     </row>
-    <row r="37" spans="5:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="5"/>
-    </row>
-    <row r="38" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="R38" s="1"/>
-      <c r="S38" s="1"/>
-    </row>
-    <row r="39" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="N37" s="4"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="5"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
     </row>
-    <row r="40" spans="5:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="R40" s="1"/>
-    </row>
-    <row r="41" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="N41" s="1"/>
-    </row>
-    <row r="42" spans="5:19" x14ac:dyDescent="0.25">
+      <c r="S40" s="1"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R41" s="1"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N42" s="1"/>
     </row>
-    <row r="43" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="N43" s="6"/>
-    </row>
-    <row r="44" spans="5:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N43" s="1"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N44" s="6"/>
     </row>
-    <row r="45" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="N45" s="7"/>
-    </row>
-    <row r="46" spans="5:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N45" s="6"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N46" s="7"/>
     </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N47" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="I11:O11"/>
+    <mergeCell ref="I29:R29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>